<commit_message>
fixed unclassified not being subtracted. regenerated figures, kw, wilcoxon.
</commit_message>
<xml_diff>
--- a/utils/paper/ad_table_04062023.xlsx
+++ b/utils/paper/ad_table_04062023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valenciaem/coding/pipelines/utils/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4479F977-C362-6C4B-BF14-0D8E94977A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27DC2F5-4040-BB4D-B5A3-59552C6D45F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="2180" windowWidth="28860" windowHeight="17000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36020" yWindow="2100" windowWidth="28860" windowHeight="17000" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AD table_species" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="FPRA" sheetId="3" r:id="rId7"/>
     <sheet name="FPRA_New_Filter" sheetId="6" r:id="rId8"/>
     <sheet name="FPRA_Tidy_NF" sheetId="9" r:id="rId9"/>
+    <sheet name="Unclassified" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="50">
   <si>
     <t>CamiSim-S2</t>
   </si>
@@ -157,7 +158,40 @@
     <t>p=0.13</t>
   </si>
   <si>
-    <t>p=0.002</t>
+    <t>Unclassified</t>
+  </si>
+  <si>
+    <t>BMock12</t>
+  </si>
+  <si>
+    <t>CamiSim S1</t>
+  </si>
+  <si>
+    <t>CamiSim S2</t>
+  </si>
+  <si>
+    <t>NIST EG</t>
+  </si>
+  <si>
+    <t>NIST MIX-A</t>
+  </si>
+  <si>
+    <t>NIST MIX-B</t>
+  </si>
+  <si>
+    <t>NIST MIX-C</t>
+  </si>
+  <si>
+    <t>NIST MIX-D</t>
+  </si>
+  <si>
+    <t>Mean (%)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>p=0.001</t>
   </si>
 </sst>
 </file>
@@ -265,7 +299,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -306,9 +340,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -316,6 +347,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -655,21 +687,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
@@ -678,26 +710,26 @@
       <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27" t="s">
+      <c r="E2" s="25"/>
+      <c r="F2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27" t="s">
+      <c r="I2" s="25"/>
+      <c r="J2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27" t="s">
+      <c r="K2" s="25"/>
+      <c r="L2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="27"/>
+      <c r="M2" s="25"/>
       <c r="N2" s="10" t="s">
         <v>26</v>
       </c>
@@ -735,7 +767,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="24" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
@@ -770,7 +802,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="26"/>
+      <c r="A5" s="24"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -803,7 +835,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
+      <c r="A6" s="24"/>
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -836,7 +868,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="26"/>
+      <c r="A7" s="24"/>
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -869,7 +901,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
+      <c r="A8" s="24"/>
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -902,7 +934,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
+      <c r="A9" s="24"/>
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -935,7 +967,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="26"/>
+      <c r="A10" s="24"/>
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -968,7 +1000,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
+      <c r="A11" s="24"/>
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -1001,7 +1033,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="24" t="s">
         <v>18</v>
       </c>
       <c r="B12" t="s">
@@ -1046,7 +1078,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
+      <c r="A13" s="24"/>
       <c r="B13" t="s">
         <v>22</v>
       </c>
@@ -1089,7 +1121,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="26"/>
+      <c r="A14" s="24"/>
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1213,19 +1245,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D88F35A-77E5-3A43-BDD4-640D2A2817D5}">
-  <dimension ref="A1:N15"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11600BB-E6D9-3B44-8FF8-7C87EEE77814}">
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1242,6 +1281,1091 @@
       <c r="N1" s="27"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="27"/>
+      <c r="N2" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="17"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="23">
+        <f t="shared" ref="C4" si="0">C22</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="9">
+        <f>H22*100</f>
+        <v>1.3231678827408</v>
+      </c>
+      <c r="I4" s="9">
+        <f t="shared" ref="I4:K4" si="1">I22*100</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <f t="shared" si="1"/>
+        <v>28.527851063752902</v>
+      </c>
+      <c r="K4" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="9">
+        <f>N22*100</f>
+        <v>5.9702037892987407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="26"/>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="23">
+        <f t="shared" ref="B5:C5" si="2">C23</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="9">
+        <f t="shared" ref="H5:N5" si="3">H23*100</f>
+        <v>2.2530659379654998</v>
+      </c>
+      <c r="I5" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" si="3"/>
+        <v>0.87779108031570996</v>
+      </c>
+      <c r="K5" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="9">
+        <f t="shared" si="3"/>
+        <v>0.62617140365624191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="26"/>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="23">
+        <f t="shared" ref="B6:C6" si="4">C24</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" ref="H6:N6" si="5">H24*100</f>
+        <v>0.8454300846630699</v>
+      </c>
+      <c r="I6" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" si="5"/>
+        <v>7.6262889769520004E-2</v>
+      </c>
+      <c r="K6" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="9">
+        <f t="shared" si="5"/>
+        <v>0.18433859488651799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="26"/>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="23">
+        <f t="shared" ref="B7:C7" si="6">C25</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="9">
+        <f t="shared" ref="H7:N7" si="7">H25*100</f>
+        <v>15.699563633813099</v>
+      </c>
+      <c r="I7" s="9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="9">
+        <f t="shared" si="7"/>
+        <v>0.59205479289125995</v>
+      </c>
+      <c r="K7" s="9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="9">
+        <f t="shared" si="7"/>
+        <v>3.2583236853408719</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="26"/>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="23">
+        <f t="shared" ref="B8:C8" si="8">C26</f>
+        <v>1</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" ref="H8:N8" si="9">H26*100</f>
+        <v>3.9547581747208302</v>
+      </c>
+      <c r="I8" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" si="9"/>
+        <v>0.23922199955124002</v>
+      </c>
+      <c r="K8" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="9">
+        <f t="shared" si="9"/>
+        <v>0.83879603485441412</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="26"/>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="23">
+        <f t="shared" ref="B9:C9" si="10">C27</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" ref="H9:N9" si="11">H27*100</f>
+        <v>4.84573168657752</v>
+      </c>
+      <c r="I9" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" si="11"/>
+        <v>0.25255839466410995</v>
+      </c>
+      <c r="K9" s="9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N9" s="9">
+        <f t="shared" si="11"/>
+        <v>1.019658016248326</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="26"/>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="23">
+        <f t="shared" ref="B10:C10" si="12">C28</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="9">
+        <f t="shared" ref="H10:N10" si="13">H28*100</f>
+        <v>6.4247333073885597</v>
+      </c>
+      <c r="I10" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="9">
+        <f t="shared" si="13"/>
+        <v>0.2233973706629</v>
+      </c>
+      <c r="K10" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" s="9">
+        <f t="shared" si="13"/>
+        <v>1.3296261356102921</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="26"/>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="23">
+        <f t="shared" ref="B11:C11" si="14">C29</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" ref="H11:N11" si="15">H29*100</f>
+        <v>2.8588094513903197</v>
+      </c>
+      <c r="I11" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="9">
+        <f t="shared" si="15"/>
+        <v>0.20430336276192002</v>
+      </c>
+      <c r="K11" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N11" s="9">
+        <f t="shared" si="15"/>
+        <v>0.61262256283044791</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="23">
+        <f t="shared" ref="B12:C12" si="16">C30</f>
+        <v>5</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" ref="H12:N12" si="17">H30*100</f>
+        <v>3.0803410096828201</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" si="17"/>
+        <v>8.4854733407686594E-2</v>
+      </c>
+      <c r="J12" s="9">
+        <f t="shared" si="17"/>
+        <v>3.3404075949730099</v>
+      </c>
+      <c r="K12" s="9">
+        <f t="shared" si="17"/>
+        <v>0.11019072916611801</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N12" s="9">
+        <f t="shared" si="17"/>
+        <v>1.2841497209311659</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="26"/>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="23">
+        <f t="shared" ref="B13:C13" si="18">C31</f>
+        <v>5</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="9">
+        <f t="shared" ref="H13:N13" si="19">H31*100</f>
+        <v>7.6297499702711393</v>
+      </c>
+      <c r="I13" s="9">
+        <f t="shared" si="19"/>
+        <v>1.5464707628868601</v>
+      </c>
+      <c r="J13" s="9">
+        <f t="shared" si="19"/>
+        <v>9.5895074661977198</v>
+      </c>
+      <c r="K13" s="9">
+        <f t="shared" si="19"/>
+        <v>6.91059482255615E-2</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N13" s="9">
+        <f t="shared" si="19"/>
+        <v>3.443851487293772</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="28"/>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="23">
+        <f t="shared" ref="B14:C14" si="20">C32</f>
+        <v>6</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="9">
+        <f t="shared" ref="H14:N14" si="21">H32*100</f>
+        <v>3.2334605334740898</v>
+      </c>
+      <c r="I14" s="9">
+        <f t="shared" si="21"/>
+        <v>0.29718678155887901</v>
+      </c>
+      <c r="J14" s="9">
+        <f t="shared" si="21"/>
+        <v>12.372128806948799</v>
+      </c>
+      <c r="K14" s="9">
+        <f t="shared" si="21"/>
+        <v>0.12537521713524902</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N14" s="9">
+        <f t="shared" si="21"/>
+        <v>3.1211178680845784</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9">
+        <f t="shared" ref="B15:G15" si="22">D33</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="9">
+        <f t="shared" ref="H15:N15" si="23">H33*100</f>
+        <v>3.4732054999999997</v>
+      </c>
+      <c r="I15" s="9">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="9">
+        <f t="shared" si="23"/>
+        <v>2.8175854999999999</v>
+      </c>
+      <c r="K15" s="9">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="9">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="9">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="9">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1.3231678827408E-2</v>
+      </c>
+      <c r="J22">
+        <v>0.28527851063752901</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="N22" s="18">
+        <f>AVERAGE(D22,F22,H22,J22,L22)</f>
+        <v>5.9702037892987406E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>2.2530659379655E-2</v>
+      </c>
+      <c r="J23">
+        <v>8.7779108031570997E-3</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="N23" s="18">
+        <f t="shared" ref="N23:N32" si="24">AVERAGE(D23,F23,H23,J23,L23)</f>
+        <v>6.2617140365624196E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>8.4543008466306992E-3</v>
+      </c>
+      <c r="J24">
+        <v>7.6262889769519997E-4</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="N24" s="18">
+        <f t="shared" si="24"/>
+        <v>1.8433859488651799E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0.15699563633813099</v>
+      </c>
+      <c r="J25">
+        <v>5.9205479289125996E-3</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="N25" s="18">
+        <f t="shared" si="24"/>
+        <v>3.258323685340872E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>3.95475817472083E-2</v>
+      </c>
+      <c r="J26">
+        <v>2.3922199955124001E-3</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="N26" s="18">
+        <f t="shared" si="24"/>
+        <v>8.3879603485441413E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>4.8457316865775202E-2</v>
+      </c>
+      <c r="J27">
+        <v>2.5255839466410998E-3</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="N27" s="18">
+        <f t="shared" si="24"/>
+        <v>1.019658016248326E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>6.4247333073885596E-2</v>
+      </c>
+      <c r="J28">
+        <v>2.2339737066289999E-3</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="N28" s="18">
+        <f t="shared" si="24"/>
+        <v>1.329626135610292E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>2.8588094513903199E-2</v>
+      </c>
+      <c r="J29">
+        <v>2.0430336276192002E-3</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="N29" s="18">
+        <f t="shared" si="24"/>
+        <v>6.1262256283044795E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>3.0803410096828202E-2</v>
+      </c>
+      <c r="I30">
+        <v>8.4854733407686595E-4</v>
+      </c>
+      <c r="J30">
+        <v>3.3404075949730098E-2</v>
+      </c>
+      <c r="K30">
+        <v>1.1019072916611801E-3</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30" s="18">
+        <f t="shared" si="24"/>
+        <v>1.2841497209311659E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>7.6297499702711394E-2</v>
+      </c>
+      <c r="I31">
+        <v>1.5464707628868601E-2</v>
+      </c>
+      <c r="J31">
+        <v>9.5895074661977206E-2</v>
+      </c>
+      <c r="K31">
+        <v>6.9105948225561505E-4</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31" s="18">
+        <f t="shared" si="24"/>
+        <v>3.4438514872937719E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>3.2334605334740897E-2</v>
+      </c>
+      <c r="I32">
+        <v>2.9718678155887901E-3</v>
+      </c>
+      <c r="J32">
+        <v>0.123721288069488</v>
+      </c>
+      <c r="K32">
+        <v>1.25375217135249E-3</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32" s="18">
+        <f t="shared" si="24"/>
+        <v>3.1211178680845782E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0</v>
+      </c>
+      <c r="E33" s="9">
+        <v>0</v>
+      </c>
+      <c r="F33" s="9">
+        <v>0</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="H33" s="9">
+        <v>3.4732054999999998E-2</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0</v>
+      </c>
+      <c r="J33" s="9">
+        <v>2.8175855E-2</v>
+      </c>
+      <c r="K33" s="9">
+        <v>0</v>
+      </c>
+      <c r="L33" s="9">
+        <v>0</v>
+      </c>
+      <c r="M33" s="9">
+        <v>0</v>
+      </c>
+      <c r="N33" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D88F35A-77E5-3A43-BDD4-640D2A2817D5}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="10" t="s">
         <v>6</v>
@@ -1249,26 +2373,26 @@
       <c r="C2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27" t="s">
+      <c r="E2" s="25"/>
+      <c r="F2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27" t="s">
+      <c r="I2" s="25"/>
+      <c r="J2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27" t="s">
+      <c r="K2" s="25"/>
+      <c r="L2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="27"/>
+      <c r="M2" s="25"/>
       <c r="N2" s="10" t="s">
         <v>31</v>
       </c>
@@ -1310,7 +2434,7 @@
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="24" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
@@ -1345,7 +2469,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="26"/>
+      <c r="A5" s="24"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -1378,7 +2502,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
+      <c r="A6" s="24"/>
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -1411,7 +2535,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="26"/>
+      <c r="A7" s="24"/>
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -1444,7 +2568,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
+      <c r="A8" s="24"/>
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -1477,7 +2601,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
+      <c r="A9" s="24"/>
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -1510,7 +2634,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="26"/>
+      <c r="A10" s="24"/>
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -1543,7 +2667,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
+      <c r="A11" s="24"/>
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -1576,7 +2700,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="24" t="s">
         <v>18</v>
       </c>
       <c r="B12" t="s">
@@ -1621,7 +2745,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
+      <c r="A13" s="24"/>
       <c r="B13" t="s">
         <v>22</v>
       </c>
@@ -1664,7 +2788,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="26"/>
+      <c r="A14" s="24"/>
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -2094,21 +3218,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -2119,26 +3243,26 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="27"/>
+      <c r="J2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="K2" s="27"/>
+      <c r="L2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="29"/>
+      <c r="M2" s="27"/>
       <c r="N2" s="7" t="s">
         <v>26</v>
       </c>
@@ -2180,7 +3304,7 @@
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -2215,7 +3339,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2248,7 +3372,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -2281,7 +3405,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2314,7 +3438,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
@@ -2347,7 +3471,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2380,7 +3504,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
@@ -2413,7 +3537,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
@@ -2446,7 +3570,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="26" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -2491,7 +3615,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
@@ -2534,7 +3658,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
@@ -2668,22 +3792,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -2693,26 +3817,26 @@
       <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="27"/>
+      <c r="J2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="K2" s="27"/>
+      <c r="L2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="29"/>
+      <c r="M2" s="27"/>
       <c r="N2" s="7" t="s">
         <v>26</v>
       </c>
@@ -2754,7 +3878,7 @@
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -2789,7 +3913,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2822,7 +3946,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -2855,7 +3979,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2888,7 +4012,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
@@ -2921,7 +4045,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2954,7 +4078,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
@@ -2987,7 +4111,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
@@ -3020,7 +4144,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="26" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -3065,7 +4189,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
@@ -3108,7 +4232,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
@@ -3157,43 +4281,43 @@
       <c r="B15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="21">
         <f>AVERAGE(D4:D14)</f>
         <v>79.374063636363644</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="21">
         <f>STDEV(D4:D14)</f>
         <v>19.21201231835289</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="21">
         <f t="shared" ref="F15:L15" si="1">AVERAGE(F4:F14)</f>
         <v>84.603554545454543</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="21">
         <f>STDEV(F4:F14)</f>
         <v>14.944280532053934</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15" s="21">
         <f t="shared" si="1"/>
         <v>87.858696363636369</v>
       </c>
-      <c r="I15" s="24">
+      <c r="I15" s="21">
         <f>STDEV(H4:H14)</f>
         <v>15.572831876782846</v>
       </c>
-      <c r="J15" s="24">
+      <c r="J15" s="21">
         <f t="shared" si="1"/>
         <v>92.344500000000011</v>
       </c>
-      <c r="K15" s="24">
+      <c r="K15" s="21">
         <f>STDEV(J4:J14)</f>
         <v>14.814387637968704</v>
       </c>
-      <c r="L15" s="24">
+      <c r="L15" s="21">
         <f t="shared" si="1"/>
         <v>81.04610000000001</v>
       </c>
-      <c r="M15" s="24">
+      <c r="M15" s="21">
         <f>STDEV(L4:L14)</f>
         <v>24.699395508918805</v>
       </c>
@@ -3577,7 +4701,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView zoomScale="111" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3586,21 +4710,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -3610,26 +4734,26 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="27"/>
+      <c r="J2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="K2" s="27"/>
+      <c r="L2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="29"/>
+      <c r="M2" s="27"/>
       <c r="N2" s="7" t="s">
         <v>29</v>
       </c>
@@ -3670,7 +4794,7 @@
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -3705,7 +4829,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -3738,7 +4862,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -3771,7 +4895,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -3804,7 +4928,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
@@ -3837,7 +4961,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -3870,7 +4994,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
@@ -3903,7 +5027,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
@@ -3936,7 +5060,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="26" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -3981,7 +5105,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
@@ -4024,7 +5148,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
@@ -4146,7 +5270,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="N15" sqref="A1:N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4155,52 +5279,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="27"/>
+      <c r="J2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="K2" s="27"/>
+      <c r="L2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="25" t="s">
+      <c r="M2" s="27"/>
+      <c r="N2" s="22" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4240,11 +5364,11 @@
       <c r="N3" s="17"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
+      <c r="B4" t="s">
+        <v>39</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -4275,9 +5399,9 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
+      <c r="A5" s="26"/>
+      <c r="B5" t="s">
+        <v>40</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -4308,9 +5432,9 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
-      <c r="B6" s="3" t="s">
-        <v>0</v>
+      <c r="A6" s="26"/>
+      <c r="B6" t="s">
+        <v>41</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -4341,9 +5465,9 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
+      <c r="A7" s="26"/>
+      <c r="B7" t="s">
+        <v>42</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -4374,9 +5498,9 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
+      <c r="A8" s="26"/>
+      <c r="B8" t="s">
+        <v>43</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -4407,9 +5531,9 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
-      <c r="B9" s="3" t="s">
-        <v>1</v>
+      <c r="A9" s="26"/>
+      <c r="B9" t="s">
+        <v>44</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -4440,9 +5564,9 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
+      <c r="A10" s="26"/>
+      <c r="B10" t="s">
+        <v>45</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -4473,9 +5597,9 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
+      <c r="A11" s="26"/>
+      <c r="B11" t="s">
+        <v>46</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -4506,10 +5630,10 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>23</v>
       </c>
       <c r="C12">
@@ -4528,16 +5652,16 @@
         <v>0</v>
       </c>
       <c r="H12" s="9">
-        <v>3.2694000000000001</v>
+        <v>0.18906000000000001</v>
       </c>
       <c r="I12" s="9">
-        <v>0.115418412742508</v>
+        <v>6.5290068157415795E-2</v>
       </c>
       <c r="J12" s="9">
-        <v>4.06548</v>
+        <v>0.72507999999999995</v>
       </c>
       <c r="K12" s="9">
-        <v>9.6759841876679298E-2</v>
+        <v>8.4018075436182199E-2</v>
       </c>
       <c r="L12" s="9">
         <v>22.23968</v>
@@ -4547,12 +5671,12 @@
       </c>
       <c r="N12" s="18">
         <f t="shared" si="0"/>
-        <v>5.9168199999999995</v>
+        <v>4.6326720000000003</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" t="s">
         <v>22</v>
       </c>
       <c r="C13">
@@ -4571,16 +5695,16 @@
         <v>0</v>
       </c>
       <c r="H13" s="9">
-        <v>9.7552800000000008</v>
+        <v>2.1255199999999999</v>
       </c>
       <c r="I13" s="9">
-        <v>1.4319707528437799</v>
+        <v>0.12316530355583</v>
       </c>
       <c r="J13" s="9">
-        <v>14.06352</v>
+        <v>4.4740200000000003</v>
       </c>
       <c r="K13" s="9">
-        <v>0.115006117228606</v>
+        <v>0.100476624147112</v>
       </c>
       <c r="L13" s="9">
         <v>27.3918</v>
@@ -4590,50 +5714,50 @@
       </c>
       <c r="N13" s="18">
         <f t="shared" si="0"/>
-        <v>11.014943999999998</v>
+        <v>7.5710919999999984</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="30"/>
-      <c r="B14" s="20" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14">
         <v>6</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="9">
         <v>12.22505</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="9">
         <v>0.14297588258164401</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="9">
         <v>4.7166166666666598</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="9">
         <v>3.7888437110372701E-2</v>
       </c>
-      <c r="H14" s="22">
-        <v>9.7893166666666591</v>
-      </c>
-      <c r="I14" s="22">
-        <v>0.22282946319251901</v>
-      </c>
-      <c r="J14" s="22">
-        <v>20.190933333333302</v>
-      </c>
-      <c r="K14" s="22">
-        <v>9.3907330207320006E-2</v>
-      </c>
-      <c r="L14" s="22">
+      <c r="H14" s="9">
+        <v>6.5558666666666596</v>
+      </c>
+      <c r="I14" s="9">
+        <v>0.32088752338890703</v>
+      </c>
+      <c r="J14" s="9">
+        <v>7.8188166666666596</v>
+      </c>
+      <c r="K14" s="9">
+        <v>4.7753216296566203E-2</v>
+      </c>
+      <c r="L14" s="9">
         <v>26.144283333333298</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="9">
         <v>0.24861157991265601</v>
       </c>
       <c r="N14" s="18">
         <f t="shared" si="0"/>
-        <v>14.613239999999985</v>
+        <v>11.492126666666655</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -4641,7 +5765,7 @@
         <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D15" s="9">
         <f>AVERAGE(D4:D14)</f>
@@ -4661,19 +5785,19 @@
       </c>
       <c r="H15" s="9">
         <f>AVERAGE(H4:H14)</f>
-        <v>8.8529906060606063</v>
+        <v>7.5853951515151499</v>
       </c>
       <c r="I15" s="9">
         <f>STDEV(H4:H14)</f>
-        <v>15.313238295042975</v>
+        <v>15.556381025817624</v>
       </c>
       <c r="J15" s="9">
         <f>AVERAGE(J4:J14)</f>
-        <v>8.5413575757575728</v>
+        <v>6.2411742424242416</v>
       </c>
       <c r="K15" s="9">
         <f>STDEV(J4:J14)</f>
-        <v>11.491417793925368</v>
+        <v>10.743587270211224</v>
       </c>
       <c r="L15" s="9">
         <f>AVERAGE(L4:L14)</f>
@@ -4686,49 +5810,16 @@
       <c r="N15" s="19"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="9">
-        <f>AVERAGE(D11:D14,D5:D9)</f>
-        <v>3.5189788888888875</v>
-      </c>
-      <c r="E16" s="9">
-        <f>STDEV(D11:D14,D5:D9)</f>
-        <v>4.8906298313009859</v>
-      </c>
-      <c r="F16" s="9">
-        <f t="shared" ref="F16:L16" si="1">AVERAGE(F11:F14,F5:F9)</f>
-        <v>1.3026796296296288</v>
-      </c>
-      <c r="G16" s="9">
-        <f>STDEV(F11:F14,F5:F9)</f>
-        <v>1.969448409872985</v>
-      </c>
-      <c r="H16" s="9">
-        <f t="shared" si="1"/>
-        <v>2.7783996296296287</v>
-      </c>
-      <c r="I16" s="9">
-        <f>STDEV(H11:H14,H5:H9)</f>
-        <v>4.0993880485589411</v>
-      </c>
-      <c r="J16" s="9">
-        <f t="shared" si="1"/>
-        <v>5.2720814814814778</v>
-      </c>
-      <c r="K16" s="9">
-        <f>STDEV(J11:J14,J5:J9)</f>
-        <v>7.0209009819385928</v>
-      </c>
-      <c r="L16" s="9">
-        <f t="shared" si="1"/>
-        <v>24.066518148148148</v>
-      </c>
-      <c r="M16" s="9">
-        <f>STDEV(L11:L14,L5:L9)</f>
-        <v>8.0939601261504954</v>
-      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4750,7 +5841,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4989,11 +6080,11 @@
       </c>
       <c r="D10" s="9">
         <f>FPRA_New_Filter!H12</f>
-        <v>3.2694000000000001</v>
+        <v>0.18906000000000001</v>
       </c>
       <c r="E10" s="9">
         <f>FPRA_New_Filter!J12</f>
-        <v>4.06548</v>
+        <v>0.72507999999999995</v>
       </c>
       <c r="F10" s="9">
         <f>FPRA_New_Filter!L12</f>
@@ -5014,11 +6105,11 @@
       </c>
       <c r="D11" s="9">
         <f>FPRA_New_Filter!H13</f>
-        <v>9.7552800000000008</v>
+        <v>2.1255199999999999</v>
       </c>
       <c r="E11" s="9">
         <f>FPRA_New_Filter!J13</f>
-        <v>14.06352</v>
+        <v>4.4740200000000003</v>
       </c>
       <c r="F11" s="9">
         <f>FPRA_New_Filter!L13</f>
@@ -5039,11 +6130,11 @@
       </c>
       <c r="D12" s="9">
         <f>FPRA_New_Filter!H14</f>
-        <v>9.7893166666666591</v>
+        <v>6.5558666666666596</v>
       </c>
       <c r="E12" s="9">
         <f>FPRA_New_Filter!J14</f>
-        <v>20.190933333333302</v>
+        <v>7.8188166666666596</v>
       </c>
       <c r="F12" s="9">
         <f>FPRA_New_Filter!L14</f>

</xml_diff>

<commit_message>
fixed file structure download, added more docs
</commit_message>
<xml_diff>
--- a/utils/paper/ad_table_04062023.xlsx
+++ b/utils/paper/ad_table_04062023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valenciaem/coding/pipelines/utils/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27DC2F5-4040-BB4D-B5A3-59552C6D45F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78E2411-43D5-2242-A212-201F2D45EE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36020" yWindow="2100" windowWidth="28860" windowHeight="17000" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1250,7 +1250,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1403,7 +1403,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="23">
-        <f t="shared" ref="B5:C5" si="2">C23</f>
+        <f t="shared" ref="C5" si="2">C23</f>
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1451,7 +1451,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="23">
-        <f t="shared" ref="B6:C6" si="4">C24</f>
+        <f t="shared" ref="C6" si="4">C24</f>
         <v>1</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -1499,7 +1499,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="23">
-        <f t="shared" ref="B7:C7" si="6">C25</f>
+        <f t="shared" ref="C7" si="6">C25</f>
         <v>1</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -1547,7 +1547,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="23">
-        <f t="shared" ref="B8:C8" si="8">C26</f>
+        <f t="shared" ref="C8" si="8">C26</f>
         <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -1595,7 +1595,7 @@
         <v>44</v>
       </c>
       <c r="C9" s="23">
-        <f t="shared" ref="B9:C9" si="10">C27</f>
+        <f t="shared" ref="C9" si="10">C27</f>
         <v>1</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -1643,7 +1643,7 @@
         <v>45</v>
       </c>
       <c r="C10" s="23">
-        <f t="shared" ref="B10:C10" si="12">C28</f>
+        <f t="shared" ref="C10" si="12">C28</f>
         <v>1</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -1691,7 +1691,7 @@
         <v>46</v>
       </c>
       <c r="C11" s="23">
-        <f t="shared" ref="B11:C11" si="14">C29</f>
+        <f t="shared" ref="C11" si="14">C29</f>
         <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
@@ -1741,7 +1741,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="23">
-        <f t="shared" ref="B12:C12" si="16">C30</f>
+        <f t="shared" ref="C12" si="16">C30</f>
         <v>5</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -1789,7 +1789,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="23">
-        <f t="shared" ref="B13:C13" si="18">C31</f>
+        <f t="shared" ref="C13" si="18">C31</f>
         <v>5</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -1837,7 +1837,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="23">
-        <f t="shared" ref="B14:C14" si="20">C32</f>
+        <f t="shared" ref="C14" si="20">C32</f>
         <v>6</v>
       </c>
       <c r="D14" s="9" t="s">
@@ -1887,49 +1887,31 @@
         <v>31</v>
       </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="9">
-        <f t="shared" ref="B15:G15" si="22">D33</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="9">
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9">
+        <f t="shared" ref="E15:N15" si="22">AVERAGE(H4:H14)</f>
+        <v>4.7408010611534319</v>
+      </c>
+      <c r="I15" s="9">
+        <f>STDEV(H4:H14)</f>
+        <v>4.1655618791075328</v>
+      </c>
+      <c r="J15" s="9">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="9">
+        <v>5.1177713474990085</v>
+      </c>
+      <c r="K15" s="9">
+        <f>STDEV(J4:J14)</f>
+        <v>8.8501804269855313</v>
+      </c>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="9">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="9">
-        <f t="shared" ref="H15:N15" si="23">H33*100</f>
-        <v>3.4732054999999997</v>
-      </c>
-      <c r="I15" s="9">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="9">
-        <f t="shared" si="23"/>
-        <v>2.8175854999999999</v>
-      </c>
-      <c r="K15" s="9">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="9">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="9">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="9">
-        <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1.9717144817304879</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -1994,7 +1976,7 @@
         <v>0</v>
       </c>
       <c r="N23" s="18">
-        <f t="shared" ref="N23:N32" si="24">AVERAGE(D23,F23,H23,J23,L23)</f>
+        <f t="shared" ref="N23:N32" si="23">AVERAGE(D23,F23,H23,J23,L23)</f>
         <v>6.2617140365624196E-3</v>
       </c>
     </row>
@@ -2021,7 +2003,7 @@
         <v>0</v>
       </c>
       <c r="N24" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1.8433859488651799E-3</v>
       </c>
     </row>
@@ -2048,7 +2030,7 @@
         <v>0</v>
       </c>
       <c r="N25" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>3.258323685340872E-2</v>
       </c>
     </row>
@@ -2075,7 +2057,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>8.3879603485441413E-3</v>
       </c>
     </row>
@@ -2102,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="N27" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1.019658016248326E-2</v>
       </c>
     </row>
@@ -2129,7 +2111,7 @@
         <v>0</v>
       </c>
       <c r="N28" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1.329626135610292E-2</v>
       </c>
     </row>
@@ -2156,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="N29" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>6.1262256283044795E-3</v>
       </c>
     </row>
@@ -2198,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="N30" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1.2841497209311659E-2</v>
       </c>
     </row>
@@ -2240,7 +2222,7 @@
         <v>0</v>
       </c>
       <c r="N31" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>3.4438514872937719E-2</v>
       </c>
     </row>
@@ -2282,7 +2264,7 @@
         <v>0</v>
       </c>
       <c r="N32" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>3.1211178680845782E-2</v>
       </c>
     </row>

</xml_diff>